<commit_message>
map, stage 수치 조정
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\endgame\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D15AA16-600F-4670-B86A-EC2320833C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BE81A7-F3C6-43D3-905D-54A55F81C4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="2265" windowWidth="25770" windowHeight="11385" xr2:uid="{2DA71CDD-AD60-487C-BAF1-C87192E711FA}"/>
+    <workbookView xWindow="2640" yWindow="2640" windowWidth="25770" windowHeight="11385" xr2:uid="{2DA71CDD-AD60-487C-BAF1-C87192E711FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -618,7 +618,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -732,19 +732,19 @@
         <v>0</v>
       </c>
       <c r="E4" s="2">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F4" s="2">
         <v>30</v>
       </c>
       <c r="G4" s="2">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="H4" s="2">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I4" s="2">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:9">

</xml_diff>